<commit_message>
modify part of function
</commit_message>
<xml_diff>
--- a/data/testcases.xlsx
+++ b/data/testcases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7935" windowWidth="20400" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7935" windowWidth="20490"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="register" sheetId="1" state="visible" r:id="rId1"/>
@@ -13,14 +13,19 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="invest" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="125725" fullCalcOnLoad="1"/>
+  <calcPr calcId="144525" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="10">
+  <numFmts count="4">
+    <numFmt formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ " numFmtId="164"/>
+    <numFmt formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ " numFmtId="165"/>
+    <numFmt formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ " numFmtId="166"/>
+    <numFmt formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ " numFmtId="167"/>
+  </numFmts>
+  <fonts count="28">
     <font>
       <name val="宋体"/>
       <charset val="134"/>
@@ -46,6 +51,15 @@
       <b val="1"/>
       <color rgb="FF000000"/>
       <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <name val="宋体"/>
@@ -53,18 +67,150 @@
       <b val="1"/>
       <color rgb="FF00FF00"/>
       <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color theme="0"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <name val="宋体"/>
       <charset val="134"/>
       <b val="1"/>
-      <color rgb="FFFF0000"/>
+      <color theme="3"/>
+      <sz val="15"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color theme="1"/>
       <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <name val="宋体"/>
       <charset val="134"/>
-      <sz val="9"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="13"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="18"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -80,15 +226,201 @@
       <color rgb="00FF0000"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -149,6 +481,104 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -158,12 +588,156 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="12" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="10" fillId="24" fontId="21" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="165">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="166">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="13" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="9" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="167">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="5" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="11" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="20" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="6" fillId="4" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="20" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="18" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="24" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="0" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="0" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="8" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="12" fillId="0" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="23" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="11" fillId="19" fontId="19" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="10" fillId="19" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="8" fillId="11" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="27" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="10" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="9" fillId="0" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="7" fillId="0" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="32" fontId="23" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="31" fontId="22" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="30" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="26" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="16" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="18" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="22" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="21" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="17" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="15" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="7" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="29" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="6" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="25" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="28" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="14" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -174,9 +748,14 @@
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -186,41 +765,81 @@
     <xf applyAlignment="1" borderId="4" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf applyAlignment="1" borderId="3" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="26" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="27" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle builtinId="0" name="常规" xfId="0"/>
+    <cellStyle builtinId="7" name="货币[0]" xfId="1"/>
+    <cellStyle builtinId="38" name="20% - 强调文字颜色 3" xfId="2"/>
+    <cellStyle builtinId="20" name="输入" xfId="3"/>
+    <cellStyle builtinId="4" name="货币" xfId="4"/>
+    <cellStyle builtinId="6" name="千位分隔[0]" xfId="5"/>
+    <cellStyle builtinId="39" name="40% - 强调文字颜色 3" xfId="6"/>
+    <cellStyle builtinId="27" name="差" xfId="7"/>
+    <cellStyle builtinId="3" name="千位分隔" xfId="8"/>
+    <cellStyle builtinId="40" name="60% - 强调文字颜色 3" xfId="9"/>
+    <cellStyle builtinId="8" name="超链接" xfId="10"/>
+    <cellStyle builtinId="5" name="百分比" xfId="11"/>
+    <cellStyle builtinId="9" name="已访问的超链接" xfId="12"/>
+    <cellStyle builtinId="10" name="注释" xfId="13"/>
+    <cellStyle builtinId="36" name="60% - 强调文字颜色 2" xfId="14"/>
+    <cellStyle builtinId="19" name="标题 4" xfId="15"/>
+    <cellStyle builtinId="11" name="警告文本" xfId="16"/>
+    <cellStyle builtinId="15" name="标题" xfId="17"/>
+    <cellStyle builtinId="53" name="解释性文本" xfId="18"/>
+    <cellStyle builtinId="16" name="标题 1" xfId="19"/>
+    <cellStyle builtinId="17" name="标题 2" xfId="20"/>
+    <cellStyle builtinId="32" name="60% - 强调文字颜色 1" xfId="21"/>
+    <cellStyle builtinId="18" name="标题 3" xfId="22"/>
+    <cellStyle builtinId="44" name="60% - 强调文字颜色 4" xfId="23"/>
+    <cellStyle builtinId="21" name="输出" xfId="24"/>
+    <cellStyle builtinId="22" name="计算" xfId="25"/>
+    <cellStyle builtinId="23" name="检查单元格" xfId="26"/>
+    <cellStyle builtinId="50" name="20% - 强调文字颜色 6" xfId="27"/>
+    <cellStyle builtinId="33" name="强调文字颜色 2" xfId="28"/>
+    <cellStyle builtinId="24" name="链接单元格" xfId="29"/>
+    <cellStyle builtinId="25" name="汇总" xfId="30"/>
+    <cellStyle builtinId="26" name="好" xfId="31"/>
+    <cellStyle builtinId="28" name="适中" xfId="32"/>
+    <cellStyle builtinId="46" name="20% - 强调文字颜色 5" xfId="33"/>
+    <cellStyle builtinId="29" name="强调文字颜色 1" xfId="34"/>
+    <cellStyle builtinId="30" name="20% - 强调文字颜色 1" xfId="35"/>
+    <cellStyle builtinId="31" name="40% - 强调文字颜色 1" xfId="36"/>
+    <cellStyle builtinId="34" name="20% - 强调文字颜色 2" xfId="37"/>
+    <cellStyle builtinId="35" name="40% - 强调文字颜色 2" xfId="38"/>
+    <cellStyle builtinId="37" name="强调文字颜色 3" xfId="39"/>
+    <cellStyle builtinId="41" name="强调文字颜色 4" xfId="40"/>
+    <cellStyle builtinId="42" name="20% - 强调文字颜色 4" xfId="41"/>
+    <cellStyle builtinId="43" name="40% - 强调文字颜色 4" xfId="42"/>
+    <cellStyle builtinId="45" name="强调文字颜色 5" xfId="43"/>
+    <cellStyle builtinId="47" name="40% - 强调文字颜色 5" xfId="44"/>
+    <cellStyle builtinId="48" name="60% - 强调文字颜色 5" xfId="45"/>
+    <cellStyle builtinId="49" name="强调文字颜色 6" xfId="46"/>
+    <cellStyle builtinId="51" name="40% - 强调文字颜色 6" xfId="47"/>
+    <cellStyle builtinId="52" name="60% - 强调文字颜色 6" xfId="48"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
@@ -507,7 +1126,6 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
@@ -519,8 +1137,8 @@
   </sheetPr>
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="0"/>
@@ -589,10 +1207,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="13" t="n">
+      <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="inlineStr">
+      <c r="B2" s="15" t="inlineStr">
         <is>
           <t>手机号未被注册</t>
         </is>
@@ -609,7 +1227,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>{"mobilephone": "${MobilePhone}", "pwd": "123456", "regname": "投资者"}</t>
+          <t>{"mobilephone": "${not_exist_phone}", "pwd": "123456", "regname": "投资者"}</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
@@ -622,12 +1240,12 @@
           <t>{"status":1,"code":"10001","data":null,"msg":"注册成功"}</t>
         </is>
       </c>
-      <c r="H2" s="17" t="inlineStr">
+      <c r="H2" s="16" t="inlineStr">
         <is>
           <t>{"status":1,"code":"10001","data":null,"msg":"注册成功"}</t>
         </is>
       </c>
-      <c r="I2" s="18" t="inlineStr">
+      <c r="I2" s="17" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
@@ -635,10 +1253,10 @@
       <c r="J2" s="2" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="13" t="n">
+      <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="inlineStr">
+      <c r="B3" s="15" t="inlineStr">
         <is>
           <t>手机号未被注册</t>
         </is>
@@ -655,7 +1273,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>{"mobilephone": "${MobilePhone}", "pwd": "12345678", "regname": "借款人"}</t>
+          <t>{"mobilephone": "${not_exist_phone}", "pwd": "12345678", "regname": "借款人"}</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
@@ -668,12 +1286,12 @@
           <t>{"status":1,"code":"10001","data":null,"msg":"注册成功"}</t>
         </is>
       </c>
-      <c r="H3" s="17" t="inlineStr">
+      <c r="H3" s="16" t="inlineStr">
         <is>
           <t>{"status":1,"code":"10001","data":null,"msg":"注册成功"}</t>
         </is>
       </c>
-      <c r="I3" s="18" t="inlineStr">
+      <c r="I3" s="17" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
@@ -681,10 +1299,10 @@
       <c r="J3" s="2" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="13" t="n">
+      <c r="A4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="inlineStr">
+      <c r="B4" s="15" t="inlineStr">
         <is>
           <t>手机号未被注册</t>
         </is>
@@ -701,7 +1319,7 @@
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>{"mobilephone": "${MobilePhone}", "pwd": "123456789012345678", "regname": "管理员"}</t>
+          <t>{"mobilephone": "${not_exist_phone}", "pwd": "123456789012345678", "regname": "管理员"}</t>
         </is>
       </c>
       <c r="F4" s="2" t="inlineStr">
@@ -714,12 +1332,12 @@
           <t>{"status":1,"code":"10001","data":null,"msg":"注册成功"}</t>
         </is>
       </c>
-      <c r="H4" s="17" t="inlineStr">
+      <c r="H4" s="16" t="inlineStr">
         <is>
           <t>{"status":1,"code":"10001","data":null,"msg":"注册成功"}</t>
         </is>
       </c>
-      <c r="I4" s="18" t="inlineStr">
+      <c r="I4" s="17" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
@@ -727,10 +1345,10 @@
       <c r="J4" s="2" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="13" t="n">
+      <c r="A5" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="inlineStr">
+      <c r="B5" s="15" t="inlineStr">
         <is>
           <t>手机号未被注册</t>
         </is>
@@ -747,7 +1365,7 @@
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>{"mobilephone": "${MobilePhone}", "pwd": "123456"}</t>
+          <t>{"mobilephone": "${not_exist_phone}", "pwd": "123456"}</t>
         </is>
       </c>
       <c r="F5" s="2" t="inlineStr">
@@ -760,12 +1378,12 @@
           <t>{"status":1,"code":"10001","data":null,"msg":"注册成功"}</t>
         </is>
       </c>
-      <c r="H5" s="17" t="inlineStr">
+      <c r="H5" s="16" t="inlineStr">
         <is>
           <t>{"status":1,"code":"10001","data":null,"msg":"注册成功"}</t>
         </is>
       </c>
-      <c r="I5" s="18" t="inlineStr">
+      <c r="I5" s="17" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
@@ -773,10 +1391,10 @@
       <c r="J5" s="2" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="13" t="n">
+      <c r="A6" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="inlineStr">
+      <c r="B6" s="15" t="inlineStr">
         <is>
           <t>手机号未被注册</t>
         </is>
@@ -793,7 +1411,7 @@
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>{"mobilephone": "${MobilePhone}", "pwd": "123456", "regname": null}</t>
+          <t>{"mobilephone": "${not_exist_phone}", "pwd": "123456", "regname": null}</t>
         </is>
       </c>
       <c r="F6" s="2" t="inlineStr">
@@ -806,12 +1424,12 @@
           <t>{"status":1,"code":"10001","data":null,"msg":"注册成功"}</t>
         </is>
       </c>
-      <c r="H6" s="17" t="inlineStr">
+      <c r="H6" s="16" t="inlineStr">
         <is>
           <t>{"status":1,"code":"10001","data":null,"msg":"注册成功"}</t>
         </is>
       </c>
-      <c r="I6" s="18" t="inlineStr">
+      <c r="I6" s="17" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
@@ -819,10 +1437,10 @@
       <c r="J6" s="2" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="13" t="n">
+      <c r="A7" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="inlineStr">
+      <c r="B7" s="15" t="inlineStr">
         <is>
           <t>手机号未被注册</t>
         </is>
@@ -852,12 +1470,12 @@
           <t>{"status":0,"code":"20103","data":null,"msg":"手机号不能为空"}</t>
         </is>
       </c>
-      <c r="H7" s="17" t="inlineStr">
+      <c r="H7" s="16" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20103","data":null,"msg":"手机号不能为空"}</t>
         </is>
       </c>
-      <c r="I7" s="18" t="inlineStr">
+      <c r="I7" s="17" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
@@ -865,10 +1483,10 @@
       <c r="J7" s="2" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="13" t="n">
+      <c r="A8" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="inlineStr">
+      <c r="B8" s="15" t="inlineStr">
         <is>
           <t>手机号未被注册</t>
         </is>
@@ -885,7 +1503,7 @@
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>{"mobilephone": "${MobilePhone}", "regname": "linux7"}</t>
+          <t>{"mobilephone": "${not_exist_phone}", "regname": "linux7"}</t>
         </is>
       </c>
       <c r="F8" s="2" t="inlineStr">
@@ -898,12 +1516,12 @@
           <t>{"status":0,"code":"20103","data":null,"msg":"密码不能为空"}</t>
         </is>
       </c>
-      <c r="H8" s="17" t="inlineStr">
+      <c r="H8" s="16" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20103","data":null,"msg":"密码不能为空"}</t>
         </is>
       </c>
-      <c r="I8" s="18" t="inlineStr">
+      <c r="I8" s="17" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
@@ -911,10 +1529,10 @@
       <c r="J8" s="2" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="13" t="n">
+      <c r="A9" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="9" t="inlineStr">
+      <c r="B9" s="15" t="inlineStr">
         <is>
           <t>手机号未被注册</t>
         </is>
@@ -931,7 +1549,7 @@
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>{"mobilephone": [${MobilePhone}], "pwd": "123456", "regname": "linux8"}</t>
+          <t>{"mobilephone": [${not_exist_phone}], "pwd": "123456", "regname": "linux8"}</t>
         </is>
       </c>
       <c r="F9" s="2" t="inlineStr">
@@ -944,12 +1562,12 @@
           <t>{"status": 0, "code": "20103", "data": null, "msg": "手机号类型错误"}</t>
         </is>
       </c>
-      <c r="H9" s="17" t="inlineStr">
+      <c r="H9" s="16" t="inlineStr">
         <is>
           <t>{"status":1,"code":"10001","data":null,"msg":"注册成功"}</t>
         </is>
       </c>
-      <c r="I9" s="19" t="inlineStr">
+      <c r="I9" s="18" t="inlineStr">
         <is>
           <t>FAIL</t>
         </is>
@@ -957,10 +1575,10 @@
       <c r="J9" s="2" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="13" t="n">
+      <c r="A10" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="9" t="inlineStr">
+      <c r="B10" s="15" t="inlineStr">
         <is>
           <t>手机号未被注册</t>
         </is>
@@ -977,7 +1595,7 @@
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>{"mobilephone": "${MobilePhone}", "pwd": 123456, "regname": "linux9"}</t>
+          <t>{"mobilephone": "${not_exist_phone}", "pwd": 123456, "regname": "linux9"}</t>
         </is>
       </c>
       <c r="F10" s="2" t="inlineStr">
@@ -990,12 +1608,12 @@
           <t>{"status": 0, "code": "20103", "data": null, "msg": "密码类型错误"}</t>
         </is>
       </c>
-      <c r="H10" s="17" t="inlineStr">
+      <c r="H10" s="16" t="inlineStr">
         <is>
           <t>{"status":1,"code":"10001","data":null,"msg":"注册成功"}</t>
         </is>
       </c>
-      <c r="I10" s="19" t="inlineStr">
+      <c r="I10" s="18" t="inlineStr">
         <is>
           <t>FAIL</t>
         </is>
@@ -1003,10 +1621,10 @@
       <c r="J10" s="2" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="13" t="n">
+      <c r="A11" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="9" t="inlineStr">
+      <c r="B11" s="15" t="inlineStr">
         <is>
           <t>手机号未被注册</t>
         </is>
@@ -1023,7 +1641,7 @@
       </c>
       <c r="E11" s="2" t="inlineStr">
         <is>
-          <t>{"mobilephone": "${MobilePhone}", "pwd": "123456", "regname": 10}</t>
+          <t>{"mobilephone": "${not_exist_phone}", "pwd": "123456", "regname": 10}</t>
         </is>
       </c>
       <c r="F11" s="2" t="inlineStr">
@@ -1036,12 +1654,12 @@
           <t>{"status": 0, "code": "20103", "data": null, "msg": "用户名类型错误"}</t>
         </is>
       </c>
-      <c r="H11" s="17" t="inlineStr">
+      <c r="H11" s="16" t="inlineStr">
         <is>
           <t>{"status":1,"code":"10001","data":null,"msg":"注册成功"}</t>
         </is>
       </c>
-      <c r="I11" s="19" t="inlineStr">
+      <c r="I11" s="18" t="inlineStr">
         <is>
           <t>FAIL</t>
         </is>
@@ -1049,10 +1667,10 @@
       <c r="J11" s="2" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="13" t="n">
+      <c r="A12" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="9" t="inlineStr">
+      <c r="B12" s="15" t="inlineStr">
         <is>
           <t>手机号未被注册</t>
         </is>
@@ -1082,12 +1700,12 @@
           <t>{"status": 0, "code": "20109", "data": null, "msg": "手机号码格式不正确"}</t>
         </is>
       </c>
-      <c r="H12" s="17" t="inlineStr">
+      <c r="H12" s="16" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20109","data":null,"msg":"手机号码格式不正确"}</t>
         </is>
       </c>
-      <c r="I12" s="18" t="inlineStr">
+      <c r="I12" s="17" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
@@ -1095,10 +1713,10 @@
       <c r="J12" s="2" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="13" t="n">
+      <c r="A13" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="9" t="inlineStr">
+      <c r="B13" s="15" t="inlineStr">
         <is>
           <t>手机号未被注册</t>
         </is>
@@ -1128,12 +1746,12 @@
           <t>{"status": 0, "code": "20109", "data": null, "msg": "手机号码格式不正确"}</t>
         </is>
       </c>
-      <c r="H13" s="17" t="inlineStr">
+      <c r="H13" s="16" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20109","data":null,"msg":"手机号码格式不正确"}</t>
         </is>
       </c>
-      <c r="I13" s="18" t="inlineStr">
+      <c r="I13" s="17" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
@@ -1141,10 +1759,10 @@
       <c r="J13" s="2" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="13" t="n">
+      <c r="A14" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="9" t="inlineStr">
+      <c r="B14" s="15" t="inlineStr">
         <is>
           <t>手机号未被注册</t>
         </is>
@@ -1161,7 +1779,7 @@
       </c>
       <c r="E14" s="2" t="inlineStr">
         <is>
-          <t>{"mobilephone": "${MobilePhone}", "pwd": "12345", "regname": "linux13"}</t>
+          <t>{"mobilephone": "${not_exist_phone}", "pwd": "12345", "regname": "linux13"}</t>
         </is>
       </c>
       <c r="F14" s="2" t="inlineStr">
@@ -1174,12 +1792,12 @@
           <t>{"status": 0, "code": "20108", "data": null, "msg": "密码长度必须为6~18"}</t>
         </is>
       </c>
-      <c r="H14" s="17" t="inlineStr">
+      <c r="H14" s="16" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20108","data":null,"msg":"密码长度必须为6~18"}</t>
         </is>
       </c>
-      <c r="I14" s="18" t="inlineStr">
+      <c r="I14" s="17" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
@@ -1187,10 +1805,10 @@
       <c r="J14" s="2" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="13" t="n">
+      <c r="A15" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="9" t="inlineStr">
+      <c r="B15" s="15" t="inlineStr">
         <is>
           <t>手机号未被注册</t>
         </is>
@@ -1207,7 +1825,7 @@
       </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
-          <t>{"mobilephone": "${MobilePhone}", "pwd": "1234567890123456789", "regname": "linux14"}</t>
+          <t>{"mobilephone": "${not_exist_phone}", "pwd": "1234567890123456789", "regname": "linux14"}</t>
         </is>
       </c>
       <c r="F15" s="2" t="inlineStr">
@@ -1220,12 +1838,12 @@
           <t>{"status": 0, "code": "20108", "data": null, "msg": "密码长度必须为6~18"}</t>
         </is>
       </c>
-      <c r="H15" s="17" t="inlineStr">
+      <c r="H15" s="16" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20108","data":null,"msg":"密码长度必须为6~18"}</t>
         </is>
       </c>
-      <c r="I15" s="18" t="inlineStr">
+      <c r="I15" s="17" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
@@ -1233,10 +1851,10 @@
       <c r="J15" s="2" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="13" t="n">
+      <c r="A16" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="9" t="inlineStr">
+      <c r="B16" s="15" t="inlineStr">
         <is>
           <t>手机号未被注册</t>
         </is>
@@ -1266,12 +1884,12 @@
           <t>{"status": 0, "code": "20103", "data": null, "msg": "手机号不能为空"}</t>
         </is>
       </c>
-      <c r="H16" s="17" t="inlineStr">
+      <c r="H16" s="16" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20103","data":null,"msg":"手机号不能为空"}</t>
         </is>
       </c>
-      <c r="I16" s="18" t="inlineStr">
+      <c r="I16" s="17" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
@@ -1279,10 +1897,10 @@
       <c r="J16" s="2" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="13" t="n">
+      <c r="A17" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="9" t="inlineStr">
+      <c r="B17" s="15" t="inlineStr">
         <is>
           <t>手机号未被注册</t>
         </is>
@@ -1299,7 +1917,7 @@
       </c>
       <c r="E17" s="2" t="inlineStr">
         <is>
-          <t>{"mobilephone": "${MobilePhone}", "pwd": null, "regname": "linux16"}</t>
+          <t>{"mobilephone": "${not_exist_phone}", "pwd": null, "regname": "linux16"}</t>
         </is>
       </c>
       <c r="F17" s="2" t="inlineStr">
@@ -1312,12 +1930,12 @@
           <t>{"status": 0, "code": "20103", "data": null, "msg": "密码不能为空"}</t>
         </is>
       </c>
-      <c r="H17" s="17" t="inlineStr">
+      <c r="H17" s="16" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20103","data":null,"msg":"密码不能为空"}</t>
         </is>
       </c>
-      <c r="I17" s="18" t="inlineStr">
+      <c r="I17" s="17" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
@@ -1325,10 +1943,10 @@
       <c r="J17" s="2" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="13" t="n">
+      <c r="A18" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="9" t="inlineStr">
+      <c r="B18" s="15" t="inlineStr">
         <is>
           <t>手机号已被注册</t>
         </is>
@@ -1345,7 +1963,7 @@
       </c>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>{"mobilephone": "${MobilePhone}", "pwd": "123456", "regname": "linux17"}</t>
+          <t>{"mobilephone": "${exist_phone}", "pwd": "123456", "regname": "linux17"}</t>
         </is>
       </c>
       <c r="F18" s="2" t="inlineStr">
@@ -1358,12 +1976,12 @@
           <t>{"status": 0, "code": "20110", "data": null, "msg": "手机号码已被注册"}</t>
         </is>
       </c>
-      <c r="H18" s="17" t="inlineStr">
+      <c r="H18" s="16" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20110","data":null,"msg":"手机号码已被注册"}</t>
         </is>
       </c>
-      <c r="I18" s="18" t="inlineStr">
+      <c r="I18" s="17" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
@@ -1388,8 +2006,8 @@
   </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="0"/>
@@ -1456,10 +2074,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="13" t="n">
+      <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="inlineStr">
+      <c r="B2" s="10" t="inlineStr">
         <is>
           <t>手机号已注册</t>
         </is>
@@ -1476,7 +2094,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>{"mobilephone": "${MobilePhone}", "pwd": "123456"}</t>
+          <t>{"mobilephone": "${exist_phone}", "pwd": "123456"}</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
@@ -1489,12 +2107,12 @@
           <t>{"status": 1, "code": "10001", "data": null, "msg": "登录成功"}</t>
         </is>
       </c>
-      <c r="H2" s="17" t="inlineStr">
+      <c r="H2" s="16" t="inlineStr">
         <is>
           <t>{"status":1,"code":"10001","data":null,"msg":"登录成功"}</t>
         </is>
       </c>
-      <c r="I2" s="18" t="inlineStr">
+      <c r="I2" s="17" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
@@ -1506,10 +2124,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="13" t="n">
+      <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="inlineStr">
+      <c r="B3" s="10" t="inlineStr">
         <is>
           <t>手机号已注册</t>
         </is>
@@ -1539,12 +2157,12 @@
           <t>{"status": 0, "code": "20103", "data": null, "msg": "手机号不能为空"}</t>
         </is>
       </c>
-      <c r="H3" s="17" t="inlineStr">
+      <c r="H3" s="16" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20103","data":null,"msg":"手机号不能为空"}</t>
         </is>
       </c>
-      <c r="I3" s="18" t="inlineStr">
+      <c r="I3" s="17" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
@@ -1556,10 +2174,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="13" t="n">
+      <c r="A4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="inlineStr">
+      <c r="B4" s="10" t="inlineStr">
         <is>
           <t>手机号已注册</t>
         </is>
@@ -1576,7 +2194,7 @@
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>{"mobilephone": "${MobilePhone}"}</t>
+          <t>{"mobilephone": "${exist_phone}"}</t>
         </is>
       </c>
       <c r="F4" s="2" t="inlineStr">
@@ -1589,12 +2207,12 @@
           <t>{"status": 0, "code": "20103", "data": null, "msg": "密码不能为空"}</t>
         </is>
       </c>
-      <c r="H4" s="17" t="inlineStr">
+      <c r="H4" s="16" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20103","data":null,"msg":"密码不能为空"}</t>
         </is>
       </c>
-      <c r="I4" s="18" t="inlineStr">
+      <c r="I4" s="17" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
@@ -1606,10 +2224,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="13" t="n">
+      <c r="A5" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="inlineStr">
+      <c r="B5" s="10" t="inlineStr">
         <is>
           <t>手机号已注册</t>
         </is>
@@ -1626,7 +2244,7 @@
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>{"mobilephone": ${MobilePhone}, "pwd": "123456"}</t>
+          <t>{"mobilephone": ${exist_phone}, "pwd": "123456"}</t>
         </is>
       </c>
       <c r="F5" s="2" t="inlineStr">
@@ -1639,12 +2257,12 @@
           <t>{"status": 0, "code": "20103", "data": null, "msg": "参数类型错误"}</t>
         </is>
       </c>
-      <c r="H5" s="17" t="inlineStr">
+      <c r="H5" s="16" t="inlineStr">
         <is>
           <t>{"status":1,"code":"10001","data":null,"msg":"登录成功"}</t>
         </is>
       </c>
-      <c r="I5" s="19" t="inlineStr">
+      <c r="I5" s="18" t="inlineStr">
         <is>
           <t>FAIL</t>
         </is>
@@ -1656,10 +2274,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="13" t="n">
+      <c r="A6" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="inlineStr">
+      <c r="B6" s="10" t="inlineStr">
         <is>
           <t>手机号已注册</t>
         </is>
@@ -1676,7 +2294,7 @@
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>{"mobilephone": "${MobilePhone}", "pwd": 123456}</t>
+          <t>{"mobilephone": "${exist_phone}", "pwd": 123456}</t>
         </is>
       </c>
       <c r="F6" s="2" t="inlineStr">
@@ -1689,12 +2307,12 @@
           <t>{"status": 0, "code": "20103", "data": null, "msg": "参数类型错误"}</t>
         </is>
       </c>
-      <c r="H6" s="17" t="inlineStr">
+      <c r="H6" s="16" t="inlineStr">
         <is>
           <t>{"status":1,"code":"10001","data":null,"msg":"登录成功"}</t>
         </is>
       </c>
-      <c r="I6" s="19" t="inlineStr">
+      <c r="I6" s="18" t="inlineStr">
         <is>
           <t>FAIL</t>
         </is>
@@ -1706,10 +2324,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="13" t="n">
+      <c r="A7" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="inlineStr">
+      <c r="B7" s="10" t="inlineStr">
         <is>
           <t>手机号已注册</t>
         </is>
@@ -1739,12 +2357,12 @@
           <t>{"status": 0, "code": "20111", "data": null, "msg": "用户名或密码错误"}</t>
         </is>
       </c>
-      <c r="H7" s="17" t="inlineStr">
+      <c r="H7" s="16" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20111","data":null,"msg":"用户名或密码错误"}</t>
         </is>
       </c>
-      <c r="I7" s="18" t="inlineStr">
+      <c r="I7" s="17" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
@@ -1756,10 +2374,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="13" t="n">
+      <c r="A8" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="inlineStr">
+      <c r="B8" s="10" t="inlineStr">
         <is>
           <t>手机号已注册</t>
         </is>
@@ -1776,7 +2394,7 @@
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>{"mobilephone": "${MobilePhone}", "pwd": "12345"}</t>
+          <t>{"mobilephone": "${exist_phone}", "pwd": "12345"}</t>
         </is>
       </c>
       <c r="F8" s="2" t="inlineStr">
@@ -1789,12 +2407,12 @@
           <t>{"status": 0, "code": "20111", "data": null, "msg": "用户名或密码错误"}</t>
         </is>
       </c>
-      <c r="H8" s="17" t="inlineStr">
+      <c r="H8" s="16" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20111","data":null,"msg":"用户名或密码错误"}</t>
         </is>
       </c>
-      <c r="I8" s="18" t="inlineStr">
+      <c r="I8" s="17" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
@@ -1806,10 +2424,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="13" t="n">
+      <c r="A9" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="7" t="inlineStr">
+      <c r="B9" s="10" t="inlineStr">
         <is>
           <t>手机号已注册</t>
         </is>
@@ -1839,12 +2457,12 @@
           <t>{"status": 0, "code": "20103", "data": null, "msg": "手机号不能为空"}</t>
         </is>
       </c>
-      <c r="H9" s="17" t="inlineStr">
+      <c r="H9" s="16" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20103","data":null,"msg":"手机号不能为空"}</t>
         </is>
       </c>
-      <c r="I9" s="18" t="inlineStr">
+      <c r="I9" s="17" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
@@ -1856,10 +2474,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="13" t="n">
+      <c r="A10" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="inlineStr">
+      <c r="B10" s="10" t="inlineStr">
         <is>
           <t>手机号已注册</t>
         </is>
@@ -1876,7 +2494,7 @@
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>{"mobilephone": "${MobilePhone}", "pwd": null}</t>
+          <t>{"mobilephone": "${exist_phone}", "pwd": null}</t>
         </is>
       </c>
       <c r="F10" s="2" t="inlineStr">
@@ -1889,12 +2507,12 @@
           <t>{"status": 0, "code": "20103", "data": null, "msg": "密码不能为空"}</t>
         </is>
       </c>
-      <c r="H10" s="17" t="inlineStr">
+      <c r="H10" s="16" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20103","data":null,"msg":"密码不能为空"}</t>
         </is>
       </c>
-      <c r="I10" s="18" t="inlineStr">
+      <c r="I10" s="17" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
@@ -1906,10 +2524,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="13" t="n">
+      <c r="A11" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="inlineStr">
+      <c r="B11" s="12" t="inlineStr">
         <is>
           <t>手机号未注册</t>
         </is>
@@ -1926,7 +2544,7 @@
       </c>
       <c r="E11" s="2" t="inlineStr">
         <is>
-          <t>{"mobilephone": "${MobilePhone}", "pwd": "123456"}</t>
+          <t>{"mobilephone": "${not_exist_phone}", "pwd": "123456"}</t>
         </is>
       </c>
       <c r="F11" s="2" t="inlineStr">
@@ -1939,12 +2557,12 @@
           <t>{"status": 0, "code": "20111", "data": null, "msg": "用户名或密码错误"}</t>
         </is>
       </c>
-      <c r="H11" s="17" t="inlineStr">
+      <c r="H11" s="16" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20111","data":null,"msg":"用户名或密码错误"}</t>
         </is>
       </c>
-      <c r="I11" s="18" t="inlineStr">
+      <c r="I11" s="17" t="inlineStr">
         <is>
           <t>PASS</t>
         </is>
@@ -2034,10 +2652,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="13" t="n">
+      <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>用户已登录</t>
         </is>
@@ -2076,10 +2694,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="13" t="n">
+      <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="n"/>
+      <c r="B3" s="5" t="n"/>
       <c r="C3" s="2" t="inlineStr">
         <is>
           <t>充值成功-充值金额为500000</t>
@@ -2114,10 +2732,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="13" t="n">
+      <c r="A4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="n"/>
+      <c r="B4" s="5" t="n"/>
       <c r="C4" s="2" t="inlineStr">
         <is>
           <t>充值成功-充值金额精度等于2</t>
@@ -2152,10 +2770,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="13" t="n">
+      <c r="A5" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="n"/>
+      <c r="B5" s="5" t="n"/>
       <c r="C5" s="2" t="inlineStr">
         <is>
           <t>充值失败-充值金额缺失</t>
@@ -2190,10 +2808,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="13" t="n">
+      <c r="A6" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="n"/>
+      <c r="B6" s="5" t="n"/>
       <c r="C6" s="2" t="inlineStr">
         <is>
           <t>充值失败-手机号缺失</t>
@@ -2228,10 +2846,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="13" t="n">
+      <c r="A7" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="14" t="n"/>
+      <c r="B7" s="5" t="n"/>
       <c r="C7" s="2" t="inlineStr">
         <is>
           <t>充值失败-充值金额类型非double</t>
@@ -2266,10 +2884,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="13" t="n">
+      <c r="A8" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="14" t="n"/>
+      <c r="B8" s="5" t="n"/>
       <c r="C8" s="2" t="inlineStr">
         <is>
           <t>充值失败-手机号类型非string</t>
@@ -2304,10 +2922,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="13" t="n">
+      <c r="A9" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="14" t="n"/>
+      <c r="B9" s="5" t="n"/>
       <c r="C9" s="2" t="inlineStr">
         <is>
           <t>充值失败-充值金额小于0</t>
@@ -2342,10 +2960,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="13" t="n">
+      <c r="A10" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="14" t="n"/>
+      <c r="B10" s="5" t="n"/>
       <c r="C10" s="2" t="inlineStr">
         <is>
           <t>充值失败-充值金额等于0</t>
@@ -2380,10 +2998,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="13" t="n">
+      <c r="A11" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="14" t="n"/>
+      <c r="B11" s="5" t="n"/>
       <c r="C11" s="2" t="inlineStr">
         <is>
           <t>充值失败-充值金额大于500000</t>
@@ -2418,10 +3036,10 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="13" t="n">
+      <c r="A12" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="14" t="n"/>
+      <c r="B12" s="5" t="n"/>
       <c r="C12" s="2" t="inlineStr">
         <is>
           <t>充值失败-充值金额精度大于2</t>
@@ -2456,10 +3074,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="13" t="n">
+      <c r="A13" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="14" t="n"/>
+      <c r="B13" s="5" t="n"/>
       <c r="C13" s="2" t="inlineStr">
         <is>
           <t>充值失败-手机号为空</t>
@@ -2494,10 +3112,10 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="13" t="n">
+      <c r="A14" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="15" t="n"/>
+      <c r="B14" s="7" t="n"/>
       <c r="C14" s="2" t="inlineStr">
         <is>
           <t>充值失败-充值金额为空</t>
@@ -2532,10 +3150,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="13" t="n">
+      <c r="A15" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="13" t="inlineStr">
+      <c r="B15" s="3" t="inlineStr">
         <is>
           <t>用户未登录</t>
         </is>
@@ -2598,11 +3216,11 @@
   <cols>
     <col customWidth="1" max="1" min="1" style="1" width="6.375"/>
     <col customWidth="1" max="2" min="2" style="1" width="23.875"/>
-    <col customWidth="1" max="3" min="3" style="5" width="43.875"/>
-    <col customWidth="1" max="4" min="4" style="5" width="8.75"/>
-    <col customWidth="1" max="5" min="5" style="5" width="128.75"/>
+    <col customWidth="1" max="3" min="3" style="8" width="43.875"/>
+    <col customWidth="1" max="4" min="4" style="8" width="8.75"/>
+    <col customWidth="1" max="5" min="5" style="8" width="128.75"/>
     <col customWidth="1" max="6" min="6" style="1" width="7.25"/>
-    <col customWidth="1" max="7" min="7" style="5" width="95.875"/>
+    <col customWidth="1" max="7" min="7" style="8" width="95.875"/>
     <col customWidth="1" max="8" min="8" style="1" width="6"/>
     <col customWidth="1" max="9" min="9" style="1" width="5.875"/>
     <col customWidth="1" max="10" min="10" style="1" width="46"/>
@@ -2661,10 +3279,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="13" t="n">
+      <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>用户ID已存在</t>
         </is>
@@ -2703,10 +3321,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="13" t="n">
+      <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="n"/>
+      <c r="B3" s="5" t="n"/>
       <c r="C3" s="2" t="inlineStr">
         <is>
           <t>加标成功-年利率大于0小于24</t>
@@ -2741,10 +3359,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="13" t="n">
+      <c r="A4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="n"/>
+      <c r="B4" s="5" t="n"/>
       <c r="C4" s="2" t="inlineStr">
         <is>
           <t>加标成功-年利率等于24</t>
@@ -2779,10 +3397,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="13" t="n">
+      <c r="A5" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="n"/>
+      <c r="B5" s="5" t="n"/>
       <c r="C5" s="2" t="inlineStr">
         <is>
           <t>加标成功-借款期限类型为0</t>
@@ -2817,10 +3435,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="13" t="n">
+      <c r="A6" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="n"/>
+      <c r="B6" s="5" t="n"/>
       <c r="C6" s="2" t="inlineStr">
         <is>
           <t>加标成功-借款期限类型为2</t>
@@ -2855,10 +3473,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="13" t="n">
+      <c r="A7" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="14" t="n"/>
+      <c r="B7" s="5" t="n"/>
       <c r="C7" s="2" t="inlineStr">
         <is>
           <t>加标成功-借款期限类型值为4</t>
@@ -2893,10 +3511,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="13" t="n">
+      <c r="A8" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="14" t="n"/>
+      <c r="B8" s="5" t="n"/>
       <c r="C8" s="2" t="inlineStr">
         <is>
           <t>加标成功-还款方式为4</t>
@@ -2931,10 +3549,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="13" t="n">
+      <c r="A9" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="14" t="n"/>
+      <c r="B9" s="5" t="n"/>
       <c r="C9" s="2" t="inlineStr">
         <is>
           <t>加标成功-还款方式为5</t>
@@ -2969,10 +3587,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="13" t="n">
+      <c r="A10" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="14" t="n"/>
+      <c r="B10" s="5" t="n"/>
       <c r="C10" s="2" t="inlineStr">
         <is>
           <t>加标成功-还款方式为10</t>
@@ -3007,10 +3625,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="13" t="n">
+      <c r="A11" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="14" t="n"/>
+      <c r="B11" s="5" t="n"/>
       <c r="C11" s="2" t="inlineStr">
         <is>
           <t>加标成功-还款方式为11</t>
@@ -3045,10 +3663,10 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="13" t="n">
+      <c r="A12" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="14" t="n"/>
+      <c r="B12" s="5" t="n"/>
       <c r="C12" s="2" t="inlineStr">
         <is>
           <t>加标成功-竞标天数为1</t>
@@ -3083,10 +3701,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="13" t="n">
+      <c r="A13" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="14" t="n"/>
+      <c r="B13" s="5" t="n"/>
       <c r="C13" s="2" t="inlineStr">
         <is>
           <t>加标成功-竞标天数为10</t>
@@ -3121,10 +3739,10 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="13" t="n">
+      <c r="A14" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="14" t="n"/>
+      <c r="B14" s="5" t="n"/>
       <c r="C14" s="2" t="inlineStr">
         <is>
           <t>加标成功-竞标天数为大于1小于10</t>
@@ -3159,10 +3777,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="13" t="n">
+      <c r="A15" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="14" t="n"/>
+      <c r="B15" s="5" t="n"/>
       <c r="C15" s="2" t="inlineStr">
         <is>
           <t>加标失败-年利率小于0</t>
@@ -3193,10 +3811,10 @@
       <c r="J15" s="2" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="13" t="n">
+      <c r="A16" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="14" t="n"/>
+      <c r="B16" s="5" t="n"/>
       <c r="C16" s="2" t="inlineStr">
         <is>
           <t>加标失败-年利率为null</t>
@@ -3217,7 +3835,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G16" s="6" t="inlineStr">
+      <c r="G16" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20103","data":null,"msg":"所有参数不能为空"}</t>
         </is>
@@ -3227,10 +3845,10 @@
       <c r="J16" s="2" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="13" t="n">
+      <c r="A17" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="14" t="n"/>
+      <c r="B17" s="5" t="n"/>
       <c r="C17" s="2" t="inlineStr">
         <is>
           <t>加标失败-年利率大于24</t>
@@ -3261,10 +3879,10 @@
       <c r="J17" s="2" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="13" t="n">
+      <c r="A18" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="14" t="n"/>
+      <c r="B18" s="5" t="n"/>
       <c r="C18" s="2" t="inlineStr">
         <is>
           <t>加标失败-年利率等于0</t>
@@ -3295,10 +3913,10 @@
       <c r="J18" s="2" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="13" t="n">
+      <c r="A19" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="14" t="n"/>
+      <c r="B19" s="5" t="n"/>
       <c r="C19" s="2" t="inlineStr">
         <is>
           <t>加标失败-借款期限类型非(0,2,4)</t>
@@ -3329,10 +3947,10 @@
       <c r="J19" s="2" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="13" t="n">
+      <c r="A20" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="14" t="n"/>
+      <c r="B20" s="5" t="n"/>
       <c r="C20" s="2" t="inlineStr">
         <is>
           <t>加标失败-借款期限类型为null</t>
@@ -3353,7 +3971,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G20" s="6" t="inlineStr">
+      <c r="G20" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20103","data":null,"msg":"所有参数不能为空"}</t>
         </is>
@@ -3363,10 +3981,10 @@
       <c r="J20" s="2" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="13" t="n">
+      <c r="A21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="14" t="n"/>
+      <c r="B21" s="5" t="n"/>
       <c r="C21" s="2" t="inlineStr">
         <is>
           <t>加标失败-还款方式非(4,5,10,11)</t>
@@ -3387,7 +4005,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G21" s="6" t="inlineStr">
+      <c r="G21" s="9" t="inlineStr">
         <is>
           <t>{"status": 0, "code": "20109", "data": null, "msg": "参数错误：还款方式类型repaymemtWay只能为4,5,10,11"}</t>
         </is>
@@ -3397,10 +4015,10 @@
       <c r="J21" s="2" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="13" t="n">
+      <c r="A22" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="14" t="n"/>
+      <c r="B22" s="5" t="n"/>
       <c r="C22" s="2" t="inlineStr">
         <is>
           <t>加标失败-还款方式为null</t>
@@ -3421,7 +4039,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G22" s="6" t="inlineStr">
+      <c r="G22" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20103","data":null,"msg":"所有参数不能为空"}</t>
         </is>
@@ -3431,10 +4049,10 @@
       <c r="J22" s="2" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="13" t="n">
+      <c r="A23" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="14" t="n"/>
+      <c r="B23" s="5" t="n"/>
       <c r="C23" s="2" t="inlineStr">
         <is>
           <t>加标失败-竞标天数小于1</t>
@@ -3455,7 +4073,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G23" s="6" t="inlineStr">
+      <c r="G23" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20109","data":null,"msg":"参数错误"}</t>
         </is>
@@ -3465,10 +4083,10 @@
       <c r="J23" s="2" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="13" t="n">
+      <c r="A24" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="14" t="n"/>
+      <c r="B24" s="5" t="n"/>
       <c r="C24" s="2" t="inlineStr">
         <is>
           <t>加标失败-竞标天数大于10</t>
@@ -3489,7 +4107,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G24" s="6" t="inlineStr">
+      <c r="G24" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20109","data":null,"msg":"参数错误"}</t>
         </is>
@@ -3499,10 +4117,10 @@
       <c r="J24" s="2" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="13" t="n">
+      <c r="A25" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="14" t="n"/>
+      <c r="B25" s="5" t="n"/>
       <c r="C25" s="2" t="inlineStr">
         <is>
           <t>加标失败-竞标天数为null</t>
@@ -3523,7 +4141,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G25" s="6" t="inlineStr">
+      <c r="G25" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20103","data":null,"msg":"所有参数不能为空"}</t>
         </is>
@@ -3533,10 +4151,10 @@
       <c r="J25" s="2" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="13" t="n">
+      <c r="A26" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="14" t="n"/>
+      <c r="B26" s="5" t="n"/>
       <c r="C26" s="2" t="inlineStr">
         <is>
           <t>加标失败-借款金额等于1000</t>
@@ -3567,10 +4185,10 @@
       <c r="J26" s="2" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="13" t="n">
+      <c r="A27" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="14" t="n"/>
+      <c r="B27" s="5" t="n"/>
       <c r="C27" s="2" t="inlineStr">
         <is>
           <t>加标失败-借款金额大于1000但不能被100整除</t>
@@ -3601,10 +4219,10 @@
       <c r="J27" s="2" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="13" t="n">
+      <c r="A28" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="14" t="n"/>
+      <c r="B28" s="5" t="n"/>
       <c r="C28" s="2" t="inlineStr">
         <is>
           <t>加标失败-借款金额为空</t>
@@ -3625,7 +4243,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G28" s="6" t="inlineStr">
+      <c r="G28" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20115","data":null,"msg":"请输入金额"}</t>
         </is>
@@ -3635,10 +4253,10 @@
       <c r="J28" s="2" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="13" t="n">
+      <c r="A29" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="14" t="n"/>
+      <c r="B29" s="5" t="n"/>
       <c r="C29" s="2" t="inlineStr">
         <is>
           <t>加标失败-用户ID缺失</t>
@@ -3659,7 +4277,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G29" s="6" t="inlineStr">
+      <c r="G29" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20103","data":null,"msg":"所有参数不能为空"}</t>
         </is>
@@ -3669,10 +4287,10 @@
       <c r="J29" s="2" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="13" t="n">
+      <c r="A30" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="14" t="n"/>
+      <c r="B30" s="5" t="n"/>
       <c r="C30" s="2" t="inlineStr">
         <is>
           <t>加标失败-标题缺失</t>
@@ -3693,7 +4311,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G30" s="6" t="inlineStr">
+      <c r="G30" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20103","data":null,"msg":"所有参数不能为空"}</t>
         </is>
@@ -3703,10 +4321,10 @@
       <c r="J30" s="2" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="13" t="n">
+      <c r="A31" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="14" t="n"/>
+      <c r="B31" s="5" t="n"/>
       <c r="C31" s="2" t="inlineStr">
         <is>
           <t>加标失败-借款金额缺失</t>
@@ -3727,7 +4345,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G31" s="6" t="inlineStr">
+      <c r="G31" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20103","data":null,"msg":"所有参数不能为空"}</t>
         </is>
@@ -3737,10 +4355,10 @@
       <c r="J31" s="2" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="13" t="n">
+      <c r="A32" s="3" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="14" t="n"/>
+      <c r="B32" s="5" t="n"/>
       <c r="C32" s="2" t="inlineStr">
         <is>
           <t>加标失败-年利率缺失</t>
@@ -3761,7 +4379,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G32" s="6" t="inlineStr">
+      <c r="G32" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20103","data":null,"msg":"所有参数不能为空"}</t>
         </is>
@@ -3771,10 +4389,10 @@
       <c r="J32" s="2" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="13" t="n">
+      <c r="A33" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="14" t="n"/>
+      <c r="B33" s="5" t="n"/>
       <c r="C33" s="2" t="inlineStr">
         <is>
           <t>加标失败-借款期限缺失</t>
@@ -3795,7 +4413,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G33" s="6" t="inlineStr">
+      <c r="G33" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20103","data":null,"msg":"所有参数不能为空"}</t>
         </is>
@@ -3805,10 +4423,10 @@
       <c r="J33" s="2" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="13" t="n">
+      <c r="A34" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="14" t="n"/>
+      <c r="B34" s="5" t="n"/>
       <c r="C34" s="2" t="inlineStr">
         <is>
           <t>加标失败-借款期限类型缺失</t>
@@ -3829,7 +4447,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G34" s="6" t="inlineStr">
+      <c r="G34" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20103","data":null,"msg":"所有参数不能为空"}</t>
         </is>
@@ -3839,10 +4457,10 @@
       <c r="J34" s="2" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="13" t="n">
+      <c r="A35" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="14" t="n"/>
+      <c r="B35" s="5" t="n"/>
       <c r="C35" s="2" t="inlineStr">
         <is>
           <t>加标失败-还款方式缺失</t>
@@ -3863,7 +4481,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G35" s="6" t="inlineStr">
+      <c r="G35" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20103","data":null,"msg":"所有参数不能为空"}</t>
         </is>
@@ -3873,10 +4491,10 @@
       <c r="J35" s="2" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="13" t="n">
+      <c r="A36" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="14" t="n"/>
+      <c r="B36" s="5" t="n"/>
       <c r="C36" s="2" t="inlineStr">
         <is>
           <t>加标失败-竞标天数缺失</t>
@@ -3897,7 +4515,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G36" s="6" t="inlineStr">
+      <c r="G36" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20103","data":null,"msg":"所有参数不能为空"}</t>
         </is>
@@ -3907,10 +4525,10 @@
       <c r="J36" s="2" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="13" t="n">
+      <c r="A37" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="14" t="n"/>
+      <c r="B37" s="5" t="n"/>
       <c r="C37" s="2" t="inlineStr">
         <is>
           <t>加标失败-用户ID类型非int</t>
@@ -3931,7 +4549,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G37" s="6" t="inlineStr">
+      <c r="G37" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20109","data":null,"msg":"参数错误:请根据参数类型对应输入，数值类型只能输入数字"}</t>
         </is>
@@ -3941,10 +4559,10 @@
       <c r="J37" s="2" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="13" t="n">
+      <c r="A38" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="14" t="n"/>
+      <c r="B38" s="5" t="n"/>
       <c r="C38" s="2" t="inlineStr">
         <is>
           <t>加标失败-标题类型非string</t>
@@ -3965,7 +4583,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G38" s="6" t="inlineStr">
+      <c r="G38" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20109","data":null,"msg":"参数错误:请根据参数类型对应输入，数值类型只能输入数字"}</t>
         </is>
@@ -3975,10 +4593,10 @@
       <c r="J38" s="2" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="13" t="n">
+      <c r="A39" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="14" t="n"/>
+      <c r="B39" s="5" t="n"/>
       <c r="C39" s="2" t="inlineStr">
         <is>
           <t>加标失败-借款金额类型非double</t>
@@ -3999,7 +4617,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G39" s="6" t="inlineStr">
+      <c r="G39" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20109","data":null,"msg":"参数错误:请根据参数类型对应输入，数值类型只能输入数字"}</t>
         </is>
@@ -4009,10 +4627,10 @@
       <c r="J39" s="2" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="13" t="n">
+      <c r="A40" s="3" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="14" t="n"/>
+      <c r="B40" s="5" t="n"/>
       <c r="C40" s="2" t="inlineStr">
         <is>
           <t>加标失败-年利率类型非double</t>
@@ -4033,7 +4651,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G40" s="6" t="inlineStr">
+      <c r="G40" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20109","data":null,"msg":"参数错误:请根据参数类型对应输入，数值类型只能输入数字"}</t>
         </is>
@@ -4043,10 +4661,10 @@
       <c r="J40" s="2" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="13" t="n">
+      <c r="A41" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="14" t="n"/>
+      <c r="B41" s="5" t="n"/>
       <c r="C41" s="2" t="inlineStr">
         <is>
           <t>加标失败-借款期限非int</t>
@@ -4067,7 +4685,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G41" s="6" t="inlineStr">
+      <c r="G41" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20109","data":null,"msg":"参数错误:请根据参数类型对应输入，数值类型只能输入数字"}</t>
         </is>
@@ -4077,10 +4695,10 @@
       <c r="J41" s="2" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="13" t="n">
+      <c r="A42" s="3" t="n">
         <v>41</v>
       </c>
-      <c r="B42" s="14" t="n"/>
+      <c r="B42" s="5" t="n"/>
       <c r="C42" s="2" t="inlineStr">
         <is>
           <t>加标失败-借款期限类型非int</t>
@@ -4101,7 +4719,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G42" s="6" t="inlineStr">
+      <c r="G42" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20109","data":null,"msg":"参数错误:请根据参数类型对应输入，数值类型只能输入数字"}</t>
         </is>
@@ -4111,10 +4729,10 @@
       <c r="J42" s="2" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="13" t="n">
+      <c r="A43" s="3" t="n">
         <v>42</v>
       </c>
-      <c r="B43" s="14" t="n"/>
+      <c r="B43" s="5" t="n"/>
       <c r="C43" s="2" t="inlineStr">
         <is>
           <t>加标失败-还款方式类型非int</t>
@@ -4135,7 +4753,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G43" s="6" t="inlineStr">
+      <c r="G43" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20109","data":null,"msg":"参数错误:请根据参数类型对应输入，数值类型只能输入数字"}</t>
         </is>
@@ -4145,10 +4763,10 @@
       <c r="J43" s="2" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="13" t="n">
+      <c r="A44" s="3" t="n">
         <v>43</v>
       </c>
-      <c r="B44" s="14" t="n"/>
+      <c r="B44" s="5" t="n"/>
       <c r="C44" s="2" t="inlineStr">
         <is>
           <t>加标失败-竞标天数类型非int</t>
@@ -4169,7 +4787,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G44" s="6" t="inlineStr">
+      <c r="G44" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20109","data":null,"msg":"参数错误:请根据参数类型对应输入，数值类型只能输入数字"}</t>
         </is>
@@ -4179,10 +4797,10 @@
       <c r="J44" s="2" t="n"/>
     </row>
     <row r="45">
-      <c r="A45" s="13" t="n">
+      <c r="A45" s="3" t="n">
         <v>44</v>
       </c>
-      <c r="B45" s="14" t="n"/>
+      <c r="B45" s="5" t="n"/>
       <c r="C45" s="2" t="inlineStr">
         <is>
           <t>加标失败-用户ID为空</t>
@@ -4203,7 +4821,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G45" s="6" t="inlineStr">
+      <c r="G45" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20103","data":null,"msg":"所有参数不能为空"}</t>
         </is>
@@ -4213,10 +4831,10 @@
       <c r="J45" s="2" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="13" t="n">
+      <c r="A46" s="3" t="n">
         <v>45</v>
       </c>
-      <c r="B46" s="14" t="n"/>
+      <c r="B46" s="5" t="n"/>
       <c r="C46" s="2" t="inlineStr">
         <is>
           <t>加标失败-标题为空</t>
@@ -4237,7 +4855,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G46" s="6" t="inlineStr">
+      <c r="G46" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20103","data":null,"msg":"所有参数不能为空"}</t>
         </is>
@@ -4247,10 +4865,10 @@
       <c r="J46" s="2" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="13" t="n">
+      <c r="A47" s="3" t="n">
         <v>46</v>
       </c>
-      <c r="B47" s="14" t="n"/>
+      <c r="B47" s="5" t="n"/>
       <c r="C47" s="2" t="inlineStr">
         <is>
           <t>加标失败-借款期限为小数</t>
@@ -4281,10 +4899,10 @@
       <c r="J47" s="2" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="13" t="n">
+      <c r="A48" s="3" t="n">
         <v>47</v>
       </c>
-      <c r="B48" s="14" t="n"/>
+      <c r="B48" s="5" t="n"/>
       <c r="C48" s="2" t="inlineStr">
         <is>
           <t>加标失败-借款期限为0</t>
@@ -4315,10 +4933,10 @@
       <c r="J48" s="2" t="n"/>
     </row>
     <row r="49">
-      <c r="A49" s="13" t="n">
+      <c r="A49" s="3" t="n">
         <v>48</v>
       </c>
-      <c r="B49" s="15" t="n"/>
+      <c r="B49" s="7" t="n"/>
       <c r="C49" s="2" t="inlineStr">
         <is>
           <t>加标失败-借款期限为null</t>
@@ -4339,7 +4957,7 @@
           <t>post</t>
         </is>
       </c>
-      <c r="G49" s="6" t="inlineStr">
+      <c r="G49" s="9" t="inlineStr">
         <is>
           <t>{"status":0,"code":"20103","data":null,"msg":"所有参数不能为空"}</t>
         </is>
@@ -4349,10 +4967,10 @@
       <c r="J49" s="2" t="n"/>
     </row>
     <row r="50">
-      <c r="A50" s="13" t="n">
+      <c r="A50" s="3" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="13" t="inlineStr">
+      <c r="B50" s="3" t="inlineStr">
         <is>
           <t>用户ID不存在</t>
         </is>
@@ -4465,10 +5083,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="13" t="n">
+      <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="inlineStr">
+      <c r="B2" s="4" t="inlineStr">
         <is>
           <t>项目为竞标状态用户存在</t>
         </is>
@@ -4502,10 +5120,10 @@
       <c r="I2" s="2" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="13" t="n">
+      <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="n"/>
+      <c r="B3" s="5" t="n"/>
       <c r="C3" s="2" t="inlineStr">
         <is>
           <t>竞标成功-投标金额等于标余额</t>
@@ -4535,10 +5153,10 @@
       <c r="I3" s="2" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="13" t="n">
+      <c r="A4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="n"/>
+      <c r="B4" s="5" t="n"/>
       <c r="C4" s="2" t="inlineStr">
         <is>
           <t>竞标成功-投资金额小于标余额</t>
@@ -4568,10 +5186,10 @@
       <c r="I4" s="2" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="13" t="n">
+      <c r="A5" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="n"/>
+      <c r="B5" s="5" t="n"/>
       <c r="C5" s="2" t="inlineStr">
         <is>
           <t>竞标失败-帐号不传</t>
@@ -4601,10 +5219,10 @@
       <c r="I5" s="2" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="13" t="n">
+      <c r="A6" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="n"/>
+      <c r="B6" s="5" t="n"/>
       <c r="C6" s="2" t="inlineStr">
         <is>
           <t>竞标失败-密码不传</t>
@@ -4634,10 +5252,10 @@
       <c r="I6" s="2" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="13" t="n">
+      <c r="A7" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="14" t="n"/>
+      <c r="B7" s="5" t="n"/>
       <c r="C7" s="2" t="inlineStr">
         <is>
           <t>竞标失败-标id不传</t>
@@ -4667,10 +5285,10 @@
       <c r="I7" s="2" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="13" t="n">
+      <c r="A8" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="14" t="n"/>
+      <c r="B8" s="5" t="n"/>
       <c r="C8" s="2" t="inlineStr">
         <is>
           <t>竞标失败-投资金额不传</t>
@@ -4700,10 +5318,10 @@
       <c r="I8" s="2" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="13" t="n">
+      <c r="A9" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="14" t="n"/>
+      <c r="B9" s="5" t="n"/>
       <c r="C9" s="2" t="inlineStr">
         <is>
           <t>竞标失败-帐号非int类型</t>
@@ -4733,10 +5351,10 @@
       <c r="I9" s="2" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="13" t="n">
+      <c r="A10" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="14" t="n"/>
+      <c r="B10" s="5" t="n"/>
       <c r="C10" s="2" t="inlineStr">
         <is>
           <t>竞标失败-密码非string类型</t>
@@ -4766,10 +5384,10 @@
       <c r="I10" s="2" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="13" t="n">
+      <c r="A11" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="14" t="n"/>
+      <c r="B11" s="5" t="n"/>
       <c r="C11" s="2" t="inlineStr">
         <is>
           <t>竞标失败-标id非double类型</t>
@@ -4799,10 +5417,10 @@
       <c r="I11" s="2" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="13" t="n">
+      <c r="A12" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="14" t="n"/>
+      <c r="B12" s="5" t="n"/>
       <c r="C12" s="2" t="inlineStr">
         <is>
           <t>竞标失败-投资金额非double类型</t>
@@ -4832,10 +5450,10 @@
       <c r="I12" s="2" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="13" t="n">
+      <c r="A13" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="14" t="n"/>
+      <c r="B13" s="5" t="n"/>
       <c r="C13" s="2" t="inlineStr">
         <is>
           <t>竞标失败-标的为null</t>
@@ -4865,10 +5483,10 @@
       <c r="I13" s="2" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="13" t="n">
+      <c r="A14" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="14" t="n"/>
+      <c r="B14" s="5" t="n"/>
       <c r="C14" s="2" t="inlineStr">
         <is>
           <t>竞标失败-标的为0</t>
@@ -4898,10 +5516,10 @@
       <c r="I14" s="2" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="13" t="n">
+      <c r="A15" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="14" t="n"/>
+      <c r="B15" s="5" t="n"/>
       <c r="C15" s="2" t="inlineStr">
         <is>
           <t>竞标失败-标的小于0</t>
@@ -4931,10 +5549,10 @@
       <c r="I15" s="2" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="13" t="n">
+      <c r="A16" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="14" t="n"/>
+      <c r="B16" s="5" t="n"/>
       <c r="C16" s="2" t="inlineStr">
         <is>
           <t>竞标失败-用户id为null</t>
@@ -4964,10 +5582,10 @@
       <c r="I16" s="2" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="13" t="n">
+      <c r="A17" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="14" t="n"/>
+      <c r="B17" s="5" t="n"/>
       <c r="C17" s="2" t="inlineStr">
         <is>
           <t>竞标失败-用户id小于0</t>
@@ -4997,10 +5615,10 @@
       <c r="I17" s="2" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="13" t="n">
+      <c r="A18" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="14" t="n"/>
+      <c r="B18" s="5" t="n"/>
       <c r="C18" s="2" t="inlineStr">
         <is>
           <t>竞标失败-用户id为0</t>
@@ -5030,10 +5648,10 @@
       <c r="I18" s="2" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="13" t="n">
+      <c r="A19" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="14" t="n"/>
+      <c r="B19" s="5" t="n"/>
       <c r="C19" s="2" t="inlineStr">
         <is>
           <t>竞标失败-密码为null</t>
@@ -5059,14 +5677,14 @@
           <t>{"status":0,"code":"11003","data":null,"msg":"参数错误:所有参数都不能为空"}</t>
         </is>
       </c>
-      <c r="H19" s="4" t="n"/>
-      <c r="I19" s="4" t="n"/>
+      <c r="H19" s="6" t="n"/>
+      <c r="I19" s="6" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="13" t="n">
+      <c r="A20" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="14" t="n"/>
+      <c r="B20" s="5" t="n"/>
       <c r="C20" s="2" t="inlineStr">
         <is>
           <t>竞标失败-密码长度小于6位</t>
@@ -5092,14 +5710,14 @@
           <t>{"status":0,"code":"11006","data":null,"msg":"参数错误，password长度必须大于6位且小于18位"}</t>
         </is>
       </c>
-      <c r="H20" s="4" t="n"/>
-      <c r="I20" s="4" t="n"/>
+      <c r="H20" s="6" t="n"/>
+      <c r="I20" s="6" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="13" t="n">
+      <c r="A21" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="15" t="n"/>
+      <c r="B21" s="7" t="n"/>
       <c r="C21" s="2" t="inlineStr">
         <is>
           <t>竞标失败-密码长度大于18位</t>
@@ -5125,14 +5743,14 @@
           <t>{"status":0,"code":"11006","data":null,"msg":"参数错误，password长度必须大于6位且小于18位"}</t>
         </is>
       </c>
-      <c r="H21" s="4" t="n"/>
-      <c r="I21" s="4" t="n"/>
+      <c r="H21" s="6" t="n"/>
+      <c r="I21" s="6" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="13" t="n">
+      <c r="A22" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="13" t="inlineStr">
+      <c r="B22" s="3" t="inlineStr">
         <is>
           <t>用户不存在</t>
         </is>
@@ -5162,14 +5780,14 @@
           <t>{"status":0,"code":"11008","data":null,"msg":"不存在该用户"}</t>
         </is>
       </c>
-      <c r="H22" s="4" t="n"/>
-      <c r="I22" s="4" t="n"/>
+      <c r="H22" s="6" t="n"/>
+      <c r="I22" s="6" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="13" t="n">
+      <c r="A23" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="13" t="inlineStr">
+      <c r="B23" s="3" t="inlineStr">
         <is>
           <t>标的不存在</t>
         </is>
@@ -5199,14 +5817,14 @@
           <t>{"status":0,"code":"11009","data":null,"msg":"不存在该标的"}</t>
         </is>
       </c>
-      <c r="H23" s="4" t="n"/>
-      <c r="I23" s="4" t="n"/>
+      <c r="H23" s="6" t="n"/>
+      <c r="I23" s="6" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="13" t="n">
+      <c r="A24" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="13" t="inlineStr">
+      <c r="B24" s="3" t="inlineStr">
         <is>
           <t>标的非竞标状态</t>
         </is>
@@ -5236,14 +5854,14 @@
           <t>{"status":0,"code":"11010","data":null,"msg":"该标不在竞标状态中，无法完成投标"}</t>
         </is>
       </c>
-      <c r="H24" s="4" t="n"/>
-      <c r="I24" s="4" t="n"/>
+      <c r="H24" s="6" t="n"/>
+      <c r="I24" s="6" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="13" t="n">
+      <c r="A25" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="13" t="inlineStr">
+      <c r="B25" s="3" t="inlineStr">
         <is>
           <t>满标</t>
         </is>
@@ -5273,14 +5891,14 @@
           <t>{"status":0,"code":"11011","data":null,"msg":"该标已经满标，无法进行投标"}</t>
         </is>
       </c>
-      <c r="H25" s="4" t="n"/>
-      <c r="I25" s="4" t="n"/>
+      <c r="H25" s="6" t="n"/>
+      <c r="I25" s="6" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="13" t="n">
+      <c r="A26" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="13" t="inlineStr">
+      <c r="B26" s="3" t="inlineStr">
         <is>
           <t>标的金额不足</t>
         </is>
@@ -5310,8 +5928,8 @@
           <t>{"status":0,"code":"11012","data":null,"msg":"该标可投金额不足"}</t>
         </is>
       </c>
-      <c r="H26" s="4" t="n"/>
-      <c r="I26" s="4" t="n"/>
+      <c r="H26" s="6" t="n"/>
+      <c r="I26" s="6" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
log and report update
</commit_message>
<xml_diff>
--- a/data/testcases.xlsx
+++ b/data/testcases.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7935" windowWidth="20490"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="register" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="login" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="recharge" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="add" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="invest" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="register" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="login" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="recharge" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="add" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="invest" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="144525" fullCalcOnLoad="1"/>

</xml_diff>